<commit_message>
Diet proportion up to predator age 20 & fully fixed max age bit
</commit_message>
<xml_diff>
--- a/data/hake_intrasp_230808_a20.xlsx
+++ b/data/hake_intrasp_230808_a20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE28A9B-4BAC-574B-AABB-DEE9B7276343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FBD7F9-8C87-DC42-9405-C9542A7ADC10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30080" windowHeight="33340" firstSheet="7" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30080" yWindow="500" windowWidth="30080" windowHeight="33340" firstSheet="7" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -1222,7 +1222,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1251,6 +1251,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1272,7 +1279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1281,6 +1288,8 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -17552,10 +17561,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:I76"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="E105" sqref="E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19762,6 +19771,731 @@
       </c>
       <c r="I76">
         <v>2.8108313501189901E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>1</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>16</v>
+      </c>
+      <c r="F77">
+        <v>1</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>10</v>
+      </c>
+      <c r="I77">
+        <v>0.111619969468499</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>1</v>
+      </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>16</v>
+      </c>
+      <c r="F78">
+        <v>2</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>10</v>
+      </c>
+      <c r="I78" s="2">
+        <v>9.9994000359978393E-6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>1</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>16</v>
+      </c>
+      <c r="F79">
+        <v>3</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>10</v>
+      </c>
+      <c r="I79">
+        <v>2.96082235065896E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>1</v>
+      </c>
+      <c r="B80">
+        <v>1</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>16</v>
+      </c>
+      <c r="F80">
+        <v>4</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>10</v>
+      </c>
+      <c r="I80">
+        <v>3.08081515109093E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>1</v>
+      </c>
+      <c r="B81">
+        <v>1</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>16</v>
+      </c>
+      <c r="F81">
+        <v>5</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>10</v>
+      </c>
+      <c r="I81">
+        <v>2.8108313501189901E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82" s="6">
+        <v>1</v>
+      </c>
+      <c r="B82" s="6">
+        <v>1</v>
+      </c>
+      <c r="C82" s="6">
+        <v>0</v>
+      </c>
+      <c r="D82" s="6">
+        <v>0</v>
+      </c>
+      <c r="E82" s="6">
+        <v>17</v>
+      </c>
+      <c r="F82" s="6">
+        <v>1</v>
+      </c>
+      <c r="G82" s="6">
+        <v>0</v>
+      </c>
+      <c r="H82" s="6">
+        <v>10</v>
+      </c>
+      <c r="I82" s="6">
+        <v>0.11161997</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A83" s="6">
+        <v>1</v>
+      </c>
+      <c r="B83" s="6">
+        <v>1</v>
+      </c>
+      <c r="C83" s="6">
+        <v>0</v>
+      </c>
+      <c r="D83" s="6">
+        <v>0</v>
+      </c>
+      <c r="E83" s="6">
+        <v>17</v>
+      </c>
+      <c r="F83" s="6">
+        <v>2</v>
+      </c>
+      <c r="G83" s="6">
+        <v>0</v>
+      </c>
+      <c r="H83" s="6">
+        <v>10</v>
+      </c>
+      <c r="I83" s="7">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84" s="6">
+        <v>1</v>
+      </c>
+      <c r="B84" s="6">
+        <v>1</v>
+      </c>
+      <c r="C84" s="6">
+        <v>0</v>
+      </c>
+      <c r="D84" s="6">
+        <v>0</v>
+      </c>
+      <c r="E84" s="6">
+        <v>17</v>
+      </c>
+      <c r="F84" s="6">
+        <v>3</v>
+      </c>
+      <c r="G84" s="6">
+        <v>0</v>
+      </c>
+      <c r="H84" s="6">
+        <v>10</v>
+      </c>
+      <c r="I84" s="6">
+        <v>2.9608220000000001E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85" s="6">
+        <v>1</v>
+      </c>
+      <c r="B85" s="6">
+        <v>1</v>
+      </c>
+      <c r="C85" s="6">
+        <v>0</v>
+      </c>
+      <c r="D85" s="6">
+        <v>0</v>
+      </c>
+      <c r="E85" s="6">
+        <v>17</v>
+      </c>
+      <c r="F85" s="6">
+        <v>4</v>
+      </c>
+      <c r="G85" s="6">
+        <v>0</v>
+      </c>
+      <c r="H85" s="6">
+        <v>10</v>
+      </c>
+      <c r="I85" s="6">
+        <v>3.0808149999999999E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86" s="6">
+        <v>1</v>
+      </c>
+      <c r="B86" s="6">
+        <v>1</v>
+      </c>
+      <c r="C86" s="6">
+        <v>0</v>
+      </c>
+      <c r="D86" s="6">
+        <v>0</v>
+      </c>
+      <c r="E86" s="6">
+        <v>17</v>
+      </c>
+      <c r="F86" s="6">
+        <v>5</v>
+      </c>
+      <c r="G86" s="6">
+        <v>0</v>
+      </c>
+      <c r="H86" s="6">
+        <v>10</v>
+      </c>
+      <c r="I86" s="6">
+        <v>2.8108310000000001E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" s="6">
+        <v>1</v>
+      </c>
+      <c r="B87" s="6">
+        <v>1</v>
+      </c>
+      <c r="C87" s="6">
+        <v>0</v>
+      </c>
+      <c r="D87" s="6">
+        <v>0</v>
+      </c>
+      <c r="E87" s="6">
+        <v>18</v>
+      </c>
+      <c r="F87" s="6">
+        <v>1</v>
+      </c>
+      <c r="G87" s="6">
+        <v>0</v>
+      </c>
+      <c r="H87" s="6">
+        <v>10</v>
+      </c>
+      <c r="I87" s="6">
+        <v>0.11161997</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" s="6">
+        <v>1</v>
+      </c>
+      <c r="B88" s="6">
+        <v>1</v>
+      </c>
+      <c r="C88" s="6">
+        <v>0</v>
+      </c>
+      <c r="D88" s="6">
+        <v>0</v>
+      </c>
+      <c r="E88" s="6">
+        <v>18</v>
+      </c>
+      <c r="F88" s="6">
+        <v>2</v>
+      </c>
+      <c r="G88" s="6">
+        <v>0</v>
+      </c>
+      <c r="H88" s="6">
+        <v>10</v>
+      </c>
+      <c r="I88" s="7">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" s="6">
+        <v>1</v>
+      </c>
+      <c r="B89" s="6">
+        <v>1</v>
+      </c>
+      <c r="C89" s="6">
+        <v>0</v>
+      </c>
+      <c r="D89" s="6">
+        <v>0</v>
+      </c>
+      <c r="E89" s="6">
+        <v>18</v>
+      </c>
+      <c r="F89" s="6">
+        <v>3</v>
+      </c>
+      <c r="G89" s="6">
+        <v>0</v>
+      </c>
+      <c r="H89" s="6">
+        <v>10</v>
+      </c>
+      <c r="I89" s="6">
+        <v>2.9608220000000001E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A90" s="6">
+        <v>1</v>
+      </c>
+      <c r="B90" s="6">
+        <v>1</v>
+      </c>
+      <c r="C90" s="6">
+        <v>0</v>
+      </c>
+      <c r="D90" s="6">
+        <v>0</v>
+      </c>
+      <c r="E90" s="6">
+        <v>18</v>
+      </c>
+      <c r="F90" s="6">
+        <v>4</v>
+      </c>
+      <c r="G90" s="6">
+        <v>0</v>
+      </c>
+      <c r="H90" s="6">
+        <v>10</v>
+      </c>
+      <c r="I90" s="6">
+        <v>3.0808149999999999E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" s="6">
+        <v>1</v>
+      </c>
+      <c r="B91" s="6">
+        <v>1</v>
+      </c>
+      <c r="C91" s="6">
+        <v>0</v>
+      </c>
+      <c r="D91" s="6">
+        <v>0</v>
+      </c>
+      <c r="E91" s="6">
+        <v>18</v>
+      </c>
+      <c r="F91" s="6">
+        <v>5</v>
+      </c>
+      <c r="G91" s="6">
+        <v>0</v>
+      </c>
+      <c r="H91" s="6">
+        <v>10</v>
+      </c>
+      <c r="I91" s="6">
+        <v>2.8108310000000001E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A92" s="6">
+        <v>1</v>
+      </c>
+      <c r="B92" s="6">
+        <v>1</v>
+      </c>
+      <c r="C92" s="6">
+        <v>0</v>
+      </c>
+      <c r="D92" s="6">
+        <v>0</v>
+      </c>
+      <c r="E92" s="6">
+        <v>19</v>
+      </c>
+      <c r="F92" s="6">
+        <v>1</v>
+      </c>
+      <c r="G92" s="6">
+        <v>0</v>
+      </c>
+      <c r="H92" s="6">
+        <v>10</v>
+      </c>
+      <c r="I92" s="6">
+        <v>0.11161997</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A93" s="6">
+        <v>1</v>
+      </c>
+      <c r="B93" s="6">
+        <v>1</v>
+      </c>
+      <c r="C93" s="6">
+        <v>0</v>
+      </c>
+      <c r="D93" s="6">
+        <v>0</v>
+      </c>
+      <c r="E93" s="6">
+        <v>19</v>
+      </c>
+      <c r="F93" s="6">
+        <v>2</v>
+      </c>
+      <c r="G93" s="6">
+        <v>0</v>
+      </c>
+      <c r="H93" s="6">
+        <v>10</v>
+      </c>
+      <c r="I93" s="7">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A94" s="6">
+        <v>1</v>
+      </c>
+      <c r="B94" s="6">
+        <v>1</v>
+      </c>
+      <c r="C94" s="6">
+        <v>0</v>
+      </c>
+      <c r="D94" s="6">
+        <v>0</v>
+      </c>
+      <c r="E94" s="6">
+        <v>19</v>
+      </c>
+      <c r="F94" s="6">
+        <v>3</v>
+      </c>
+      <c r="G94" s="6">
+        <v>0</v>
+      </c>
+      <c r="H94" s="6">
+        <v>10</v>
+      </c>
+      <c r="I94" s="6">
+        <v>2.9608220000000001E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A95" s="6">
+        <v>1</v>
+      </c>
+      <c r="B95" s="6">
+        <v>1</v>
+      </c>
+      <c r="C95" s="6">
+        <v>0</v>
+      </c>
+      <c r="D95" s="6">
+        <v>0</v>
+      </c>
+      <c r="E95" s="6">
+        <v>19</v>
+      </c>
+      <c r="F95" s="6">
+        <v>4</v>
+      </c>
+      <c r="G95" s="6">
+        <v>0</v>
+      </c>
+      <c r="H95" s="6">
+        <v>10</v>
+      </c>
+      <c r="I95" s="6">
+        <v>3.0808149999999999E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A96" s="6">
+        <v>1</v>
+      </c>
+      <c r="B96" s="6">
+        <v>1</v>
+      </c>
+      <c r="C96" s="6">
+        <v>0</v>
+      </c>
+      <c r="D96" s="6">
+        <v>0</v>
+      </c>
+      <c r="E96" s="6">
+        <v>19</v>
+      </c>
+      <c r="F96" s="6">
+        <v>5</v>
+      </c>
+      <c r="G96" s="6">
+        <v>0</v>
+      </c>
+      <c r="H96" s="6">
+        <v>10</v>
+      </c>
+      <c r="I96" s="6">
+        <v>2.8108310000000001E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A97" s="6">
+        <v>1</v>
+      </c>
+      <c r="B97" s="6">
+        <v>1</v>
+      </c>
+      <c r="C97" s="6">
+        <v>0</v>
+      </c>
+      <c r="D97" s="6">
+        <v>0</v>
+      </c>
+      <c r="E97" s="6">
+        <v>20</v>
+      </c>
+      <c r="F97" s="6">
+        <v>1</v>
+      </c>
+      <c r="G97" s="6">
+        <v>0</v>
+      </c>
+      <c r="H97" s="6">
+        <v>10</v>
+      </c>
+      <c r="I97" s="6">
+        <v>0.11161997</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A98" s="6">
+        <v>1</v>
+      </c>
+      <c r="B98" s="6">
+        <v>1</v>
+      </c>
+      <c r="C98" s="6">
+        <v>0</v>
+      </c>
+      <c r="D98" s="6">
+        <v>0</v>
+      </c>
+      <c r="E98" s="6">
+        <v>20</v>
+      </c>
+      <c r="F98" s="6">
+        <v>2</v>
+      </c>
+      <c r="G98" s="6">
+        <v>0</v>
+      </c>
+      <c r="H98" s="6">
+        <v>10</v>
+      </c>
+      <c r="I98" s="7">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A99" s="6">
+        <v>1</v>
+      </c>
+      <c r="B99" s="6">
+        <v>1</v>
+      </c>
+      <c r="C99" s="6">
+        <v>0</v>
+      </c>
+      <c r="D99" s="6">
+        <v>0</v>
+      </c>
+      <c r="E99" s="6">
+        <v>20</v>
+      </c>
+      <c r="F99" s="6">
+        <v>3</v>
+      </c>
+      <c r="G99" s="6">
+        <v>0</v>
+      </c>
+      <c r="H99" s="6">
+        <v>10</v>
+      </c>
+      <c r="I99" s="6">
+        <v>2.9608220000000001E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A100" s="6">
+        <v>1</v>
+      </c>
+      <c r="B100" s="6">
+        <v>1</v>
+      </c>
+      <c r="C100" s="6">
+        <v>0</v>
+      </c>
+      <c r="D100" s="6">
+        <v>0</v>
+      </c>
+      <c r="E100" s="6">
+        <v>20</v>
+      </c>
+      <c r="F100" s="6">
+        <v>4</v>
+      </c>
+      <c r="G100" s="6">
+        <v>0</v>
+      </c>
+      <c r="H100" s="6">
+        <v>10</v>
+      </c>
+      <c r="I100" s="6">
+        <v>3.0808149999999999E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A101" s="6">
+        <v>1</v>
+      </c>
+      <c r="B101" s="6">
+        <v>1</v>
+      </c>
+      <c r="C101" s="6">
+        <v>0</v>
+      </c>
+      <c r="D101" s="6">
+        <v>0</v>
+      </c>
+      <c r="E101" s="6">
+        <v>20</v>
+      </c>
+      <c r="F101" s="6">
+        <v>5</v>
+      </c>
+      <c r="G101" s="6">
+        <v>0</v>
+      </c>
+      <c r="H101" s="6">
+        <v>10</v>
+      </c>
+      <c r="I101" s="6">
+        <v>2.8108310000000001E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ran models with max age = 20
</commit_message>
<xml_diff>
--- a/data/hake_intrasp_230808_a20.xlsx
+++ b/data/hake_intrasp_230808_a20.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FBD7F9-8C87-DC42-9405-C9542A7ADC10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93507F40-9DC2-F647-8B27-D10C729470FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30080" yWindow="500" windowWidth="30080" windowHeight="33340" firstSheet="7" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6380" yWindow="500" windowWidth="30080" windowHeight="33340" firstSheet="7" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -1222,7 +1222,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1251,13 +1251,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1279,7 +1272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1288,8 +1281,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -17564,7 +17555,7 @@
   <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E105" sqref="E105"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17624,7 +17615,7 @@
         <v>10</v>
       </c>
       <c r="I2">
-        <v>1.44591324520529E-2</v>
+        <v>1.7758934463932199E-2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -17769,7 +17760,7 @@
         <v>10</v>
       </c>
       <c r="I7">
-        <v>1.5301506152055101E-2</v>
+        <v>1.6564309171752702E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -17914,7 +17905,7 @@
         <v>10</v>
       </c>
       <c r="I12">
-        <v>4.3291049452121397E-3</v>
+        <v>4.8951980413245999E-3</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -18059,7 +18050,7 @@
         <v>10</v>
       </c>
       <c r="I17">
-        <v>2.05261202280889E-2</v>
+        <v>2.1227922364199001E-2</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -18204,7 +18195,7 @@
         <v>10</v>
       </c>
       <c r="I22">
-        <v>1.6733995960242401E-2</v>
+        <v>1.6484010959342401E-2</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -18349,7 +18340,7 @@
         <v>10</v>
       </c>
       <c r="I27">
-        <v>4.37863907396518E-2</v>
+        <v>4.6164319091823398E-2</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -18494,7 +18485,7 @@
         <v>10</v>
       </c>
       <c r="I32">
-        <v>0.100822541245588</v>
+        <v>0.10056272834418201</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -18639,7 +18630,7 @@
         <v>10</v>
       </c>
       <c r="I37">
-        <v>9.8968654523472893E-2</v>
+        <v>0.104964054221743</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -18668,7 +18659,7 @@
         <v>10</v>
       </c>
       <c r="I38">
-        <v>2.3098614083155002E-3</v>
+        <v>2.80983141011539E-3</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -18784,7 +18775,7 @@
         <v>10</v>
       </c>
       <c r="I42">
-        <v>0.107053576785393</v>
+        <v>0.10485370877747301</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -18813,7 +18804,7 @@
         <v>10</v>
       </c>
       <c r="I43">
-        <v>1.2809231446113199E-2</v>
+        <v>1.5409075455472701E-2</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -18929,7 +18920,7 @@
         <v>10</v>
       </c>
       <c r="I47">
-        <v>7.1939016992313795E-2</v>
+        <v>6.8955862648241106E-2</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -19074,7 +19065,7 @@
         <v>10</v>
       </c>
       <c r="I52">
-        <v>0.20832212984647699</v>
+        <v>0.20816889877699599</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
@@ -19219,7 +19210,7 @@
         <v>10</v>
       </c>
       <c r="I57">
-        <v>0.10503703111146701</v>
+        <v>0.10502036544474</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
@@ -19248,7 +19239,7 @@
         <v>10</v>
       </c>
       <c r="I58">
-        <v>8.4571592371124396E-2</v>
+        <v>8.2955022698638095E-2</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
@@ -19364,7 +19355,7 @@
         <v>10</v>
       </c>
       <c r="I62">
-        <v>0.12675239485630899</v>
+        <v>0.12830230186188801</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
@@ -19393,7 +19384,7 @@
         <v>10</v>
       </c>
       <c r="I63">
-        <v>1.8558886466811999E-2</v>
+        <v>1.7458952462852201E-2</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
@@ -19509,7 +19500,7 @@
         <v>10</v>
       </c>
       <c r="I67">
-        <v>0.100903560477376</v>
+        <v>9.7995500123580201E-2</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
@@ -19538,7 +19529,7 @@
         <v>10</v>
       </c>
       <c r="I68">
-        <v>9.7594144351339004E-3</v>
+        <v>1.21592704437734E-2</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
@@ -19567,7 +19558,7 @@
         <v>10</v>
       </c>
       <c r="I69">
-        <v>2.45085294882307E-2</v>
+        <v>2.3608583484990901E-2</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
@@ -19625,7 +19616,7 @@
         <v>10</v>
       </c>
       <c r="I71">
-        <v>4.1759295631500298E-2</v>
+        <v>4.1619387219349602E-2</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
@@ -19654,7 +19645,7 @@
         <v>10</v>
       </c>
       <c r="I72">
-        <v>0.111619969468499</v>
+        <v>0.108620149457699</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
@@ -19712,7 +19703,7 @@
         <v>10</v>
       </c>
       <c r="I74">
-        <v>2.96082235065896E-2</v>
+        <v>3.0608163510189398E-2</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
@@ -19741,7 +19732,7 @@
         <v>10</v>
       </c>
       <c r="I75">
-        <v>3.08081515109093E-2</v>
+        <v>2.87082775033498E-2</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
@@ -19770,7 +19761,7 @@
         <v>10</v>
       </c>
       <c r="I76">
-        <v>2.8108313501189901E-2</v>
+        <v>2.9408235505869702E-2</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
@@ -19799,7 +19790,7 @@
         <v>10</v>
       </c>
       <c r="I77">
-        <v>0.111619969468499</v>
+        <v>0.108620149457699</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
@@ -19857,7 +19848,7 @@
         <v>10</v>
       </c>
       <c r="I79">
-        <v>2.96082235065896E-2</v>
+        <v>3.0608163510189398E-2</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
@@ -19886,7 +19877,7 @@
         <v>10</v>
       </c>
       <c r="I80">
-        <v>3.08081515109093E-2</v>
+        <v>2.87082775033498E-2</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
@@ -19915,587 +19906,587 @@
         <v>10</v>
       </c>
       <c r="I81">
-        <v>2.8108313501189901E-2</v>
+        <v>2.9408235505869702E-2</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A82" s="6">
-        <v>1</v>
-      </c>
-      <c r="B82" s="6">
-        <v>1</v>
-      </c>
-      <c r="C82" s="6">
-        <v>0</v>
-      </c>
-      <c r="D82" s="6">
-        <v>0</v>
-      </c>
-      <c r="E82" s="6">
+      <c r="A82">
+        <v>1</v>
+      </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
         <v>17</v>
       </c>
-      <c r="F82" s="6">
-        <v>1</v>
-      </c>
-      <c r="G82" s="6">
-        <v>0</v>
-      </c>
-      <c r="H82" s="6">
+      <c r="F82">
+        <v>1</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="H82">
         <v>10</v>
       </c>
-      <c r="I82" s="6">
-        <v>0.11161997</v>
+      <c r="I82">
+        <v>0.108620149457699</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A83" s="6">
-        <v>1</v>
-      </c>
-      <c r="B83" s="6">
-        <v>1</v>
-      </c>
-      <c r="C83" s="6">
-        <v>0</v>
-      </c>
-      <c r="D83" s="6">
-        <v>0</v>
-      </c>
-      <c r="E83" s="6">
+      <c r="A83">
+        <v>1</v>
+      </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
         <v>17</v>
       </c>
-      <c r="F83" s="6">
+      <c r="F83">
         <v>2</v>
       </c>
-      <c r="G83" s="6">
-        <v>0</v>
-      </c>
-      <c r="H83" s="6">
+      <c r="G83">
+        <v>0</v>
+      </c>
+      <c r="H83">
         <v>10</v>
       </c>
-      <c r="I83" s="7">
-        <v>1.0000000000000001E-5</v>
+      <c r="I83" s="2">
+        <v>9.9994000359978393E-6</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A84" s="6">
-        <v>1</v>
-      </c>
-      <c r="B84" s="6">
-        <v>1</v>
-      </c>
-      <c r="C84" s="6">
-        <v>0</v>
-      </c>
-      <c r="D84" s="6">
-        <v>0</v>
-      </c>
-      <c r="E84" s="6">
+      <c r="A84">
+        <v>1</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84">
         <v>17</v>
       </c>
-      <c r="F84" s="6">
+      <c r="F84">
         <v>3</v>
       </c>
-      <c r="G84" s="6">
-        <v>0</v>
-      </c>
-      <c r="H84" s="6">
+      <c r="G84">
+        <v>0</v>
+      </c>
+      <c r="H84">
         <v>10</v>
       </c>
-      <c r="I84" s="6">
-        <v>2.9608220000000001E-2</v>
+      <c r="I84">
+        <v>3.0608163510189398E-2</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A85" s="6">
-        <v>1</v>
-      </c>
-      <c r="B85" s="6">
-        <v>1</v>
-      </c>
-      <c r="C85" s="6">
-        <v>0</v>
-      </c>
-      <c r="D85" s="6">
-        <v>0</v>
-      </c>
-      <c r="E85" s="6">
+      <c r="A85">
+        <v>1</v>
+      </c>
+      <c r="B85">
+        <v>1</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
         <v>17</v>
       </c>
-      <c r="F85" s="6">
+      <c r="F85">
         <v>4</v>
       </c>
-      <c r="G85" s="6">
-        <v>0</v>
-      </c>
-      <c r="H85" s="6">
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85">
         <v>10</v>
       </c>
-      <c r="I85" s="6">
-        <v>3.0808149999999999E-2</v>
+      <c r="I85">
+        <v>2.87082775033498E-2</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A86" s="6">
-        <v>1</v>
-      </c>
-      <c r="B86" s="6">
-        <v>1</v>
-      </c>
-      <c r="C86" s="6">
-        <v>0</v>
-      </c>
-      <c r="D86" s="6">
-        <v>0</v>
-      </c>
-      <c r="E86" s="6">
+      <c r="A86">
+        <v>1</v>
+      </c>
+      <c r="B86">
+        <v>1</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
         <v>17</v>
       </c>
-      <c r="F86" s="6">
+      <c r="F86">
         <v>5</v>
       </c>
-      <c r="G86" s="6">
-        <v>0</v>
-      </c>
-      <c r="H86" s="6">
+      <c r="G86">
+        <v>0</v>
+      </c>
+      <c r="H86">
         <v>10</v>
       </c>
-      <c r="I86" s="6">
-        <v>2.8108310000000001E-2</v>
+      <c r="I86">
+        <v>2.9408235505869702E-2</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A87" s="6">
-        <v>1</v>
-      </c>
-      <c r="B87" s="6">
-        <v>1</v>
-      </c>
-      <c r="C87" s="6">
-        <v>0</v>
-      </c>
-      <c r="D87" s="6">
-        <v>0</v>
-      </c>
-      <c r="E87" s="6">
+      <c r="A87">
+        <v>1</v>
+      </c>
+      <c r="B87">
+        <v>1</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87">
         <v>18</v>
       </c>
-      <c r="F87" s="6">
-        <v>1</v>
-      </c>
-      <c r="G87" s="6">
-        <v>0</v>
-      </c>
-      <c r="H87" s="6">
+      <c r="F87">
+        <v>1</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+      <c r="H87">
         <v>10</v>
       </c>
-      <c r="I87" s="6">
-        <v>0.11161997</v>
+      <c r="I87">
+        <v>0.108620149457699</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A88" s="6">
-        <v>1</v>
-      </c>
-      <c r="B88" s="6">
-        <v>1</v>
-      </c>
-      <c r="C88" s="6">
-        <v>0</v>
-      </c>
-      <c r="D88" s="6">
-        <v>0</v>
-      </c>
-      <c r="E88" s="6">
+      <c r="A88">
+        <v>1</v>
+      </c>
+      <c r="B88">
+        <v>1</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
         <v>18</v>
       </c>
-      <c r="F88" s="6">
+      <c r="F88">
         <v>2</v>
       </c>
-      <c r="G88" s="6">
-        <v>0</v>
-      </c>
-      <c r="H88" s="6">
+      <c r="G88">
+        <v>0</v>
+      </c>
+      <c r="H88">
         <v>10</v>
       </c>
-      <c r="I88" s="7">
-        <v>1.0000000000000001E-5</v>
+      <c r="I88" s="2">
+        <v>9.9994000359978393E-6</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A89" s="6">
-        <v>1</v>
-      </c>
-      <c r="B89" s="6">
-        <v>1</v>
-      </c>
-      <c r="C89" s="6">
-        <v>0</v>
-      </c>
-      <c r="D89" s="6">
-        <v>0</v>
-      </c>
-      <c r="E89" s="6">
+      <c r="A89">
+        <v>1</v>
+      </c>
+      <c r="B89">
+        <v>1</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89">
         <v>18</v>
       </c>
-      <c r="F89" s="6">
+      <c r="F89">
         <v>3</v>
       </c>
-      <c r="G89" s="6">
-        <v>0</v>
-      </c>
-      <c r="H89" s="6">
+      <c r="G89">
+        <v>0</v>
+      </c>
+      <c r="H89">
         <v>10</v>
       </c>
-      <c r="I89" s="6">
-        <v>2.9608220000000001E-2</v>
+      <c r="I89">
+        <v>3.0608163510189398E-2</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A90" s="6">
-        <v>1</v>
-      </c>
-      <c r="B90" s="6">
-        <v>1</v>
-      </c>
-      <c r="C90" s="6">
-        <v>0</v>
-      </c>
-      <c r="D90" s="6">
-        <v>0</v>
-      </c>
-      <c r="E90" s="6">
+      <c r="A90">
+        <v>1</v>
+      </c>
+      <c r="B90">
+        <v>1</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
         <v>18</v>
       </c>
-      <c r="F90" s="6">
+      <c r="F90">
         <v>4</v>
       </c>
-      <c r="G90" s="6">
-        <v>0</v>
-      </c>
-      <c r="H90" s="6">
+      <c r="G90">
+        <v>0</v>
+      </c>
+      <c r="H90">
         <v>10</v>
       </c>
-      <c r="I90" s="6">
-        <v>3.0808149999999999E-2</v>
+      <c r="I90">
+        <v>2.87082775033498E-2</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A91" s="6">
-        <v>1</v>
-      </c>
-      <c r="B91" s="6">
-        <v>1</v>
-      </c>
-      <c r="C91" s="6">
-        <v>0</v>
-      </c>
-      <c r="D91" s="6">
-        <v>0</v>
-      </c>
-      <c r="E91" s="6">
+      <c r="A91">
+        <v>1</v>
+      </c>
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91">
         <v>18</v>
       </c>
-      <c r="F91" s="6">
+      <c r="F91">
         <v>5</v>
       </c>
-      <c r="G91" s="6">
-        <v>0</v>
-      </c>
-      <c r="H91" s="6">
+      <c r="G91">
+        <v>0</v>
+      </c>
+      <c r="H91">
         <v>10</v>
       </c>
-      <c r="I91" s="6">
-        <v>2.8108310000000001E-2</v>
+      <c r="I91">
+        <v>2.9408235505869702E-2</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A92" s="6">
-        <v>1</v>
-      </c>
-      <c r="B92" s="6">
-        <v>1</v>
-      </c>
-      <c r="C92" s="6">
-        <v>0</v>
-      </c>
-      <c r="D92" s="6">
-        <v>0</v>
-      </c>
-      <c r="E92" s="6">
+      <c r="A92">
+        <v>1</v>
+      </c>
+      <c r="B92">
+        <v>1</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92">
         <v>19</v>
       </c>
-      <c r="F92" s="6">
-        <v>1</v>
-      </c>
-      <c r="G92" s="6">
-        <v>0</v>
-      </c>
-      <c r="H92" s="6">
+      <c r="F92">
+        <v>1</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+      <c r="H92">
         <v>10</v>
       </c>
-      <c r="I92" s="6">
-        <v>0.11161997</v>
+      <c r="I92">
+        <v>0.108620149457699</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A93" s="6">
-        <v>1</v>
-      </c>
-      <c r="B93" s="6">
-        <v>1</v>
-      </c>
-      <c r="C93" s="6">
-        <v>0</v>
-      </c>
-      <c r="D93" s="6">
-        <v>0</v>
-      </c>
-      <c r="E93" s="6">
+      <c r="A93">
+        <v>1</v>
+      </c>
+      <c r="B93">
+        <v>1</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
         <v>19</v>
       </c>
-      <c r="F93" s="6">
+      <c r="F93">
         <v>2</v>
       </c>
-      <c r="G93" s="6">
-        <v>0</v>
-      </c>
-      <c r="H93" s="6">
+      <c r="G93">
+        <v>0</v>
+      </c>
+      <c r="H93">
         <v>10</v>
       </c>
-      <c r="I93" s="7">
-        <v>1.0000000000000001E-5</v>
+      <c r="I93" s="2">
+        <v>9.9994000359978393E-6</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A94" s="6">
-        <v>1</v>
-      </c>
-      <c r="B94" s="6">
-        <v>1</v>
-      </c>
-      <c r="C94" s="6">
-        <v>0</v>
-      </c>
-      <c r="D94" s="6">
-        <v>0</v>
-      </c>
-      <c r="E94" s="6">
+      <c r="A94">
+        <v>1</v>
+      </c>
+      <c r="B94">
+        <v>1</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
         <v>19</v>
       </c>
-      <c r="F94" s="6">
+      <c r="F94">
         <v>3</v>
       </c>
-      <c r="G94" s="6">
-        <v>0</v>
-      </c>
-      <c r="H94" s="6">
+      <c r="G94">
+        <v>0</v>
+      </c>
+      <c r="H94">
         <v>10</v>
       </c>
-      <c r="I94" s="6">
-        <v>2.9608220000000001E-2</v>
+      <c r="I94">
+        <v>3.0608163510189398E-2</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A95" s="6">
-        <v>1</v>
-      </c>
-      <c r="B95" s="6">
-        <v>1</v>
-      </c>
-      <c r="C95" s="6">
-        <v>0</v>
-      </c>
-      <c r="D95" s="6">
-        <v>0</v>
-      </c>
-      <c r="E95" s="6">
+      <c r="A95">
+        <v>1</v>
+      </c>
+      <c r="B95">
+        <v>1</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
         <v>19</v>
       </c>
-      <c r="F95" s="6">
+      <c r="F95">
         <v>4</v>
       </c>
-      <c r="G95" s="6">
-        <v>0</v>
-      </c>
-      <c r="H95" s="6">
+      <c r="G95">
+        <v>0</v>
+      </c>
+      <c r="H95">
         <v>10</v>
       </c>
-      <c r="I95" s="6">
-        <v>3.0808149999999999E-2</v>
+      <c r="I95">
+        <v>2.87082775033498E-2</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A96" s="6">
-        <v>1</v>
-      </c>
-      <c r="B96" s="6">
-        <v>1</v>
-      </c>
-      <c r="C96" s="6">
-        <v>0</v>
-      </c>
-      <c r="D96" s="6">
-        <v>0</v>
-      </c>
-      <c r="E96" s="6">
+      <c r="A96">
+        <v>1</v>
+      </c>
+      <c r="B96">
+        <v>1</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
         <v>19</v>
       </c>
-      <c r="F96" s="6">
+      <c r="F96">
         <v>5</v>
       </c>
-      <c r="G96" s="6">
-        <v>0</v>
-      </c>
-      <c r="H96" s="6">
+      <c r="G96">
+        <v>0</v>
+      </c>
+      <c r="H96">
         <v>10</v>
       </c>
-      <c r="I96" s="6">
-        <v>2.8108310000000001E-2</v>
+      <c r="I96">
+        <v>2.9408235505869702E-2</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A97" s="6">
-        <v>1</v>
-      </c>
-      <c r="B97" s="6">
-        <v>1</v>
-      </c>
-      <c r="C97" s="6">
-        <v>0</v>
-      </c>
-      <c r="D97" s="6">
-        <v>0</v>
-      </c>
-      <c r="E97" s="6">
+      <c r="A97">
+        <v>1</v>
+      </c>
+      <c r="B97">
+        <v>1</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
         <v>20</v>
       </c>
-      <c r="F97" s="6">
-        <v>1</v>
-      </c>
-      <c r="G97" s="6">
-        <v>0</v>
-      </c>
-      <c r="H97" s="6">
+      <c r="F97">
+        <v>1</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+      <c r="H97">
         <v>10</v>
       </c>
-      <c r="I97" s="6">
-        <v>0.11161997</v>
+      <c r="I97">
+        <v>0.108620149457699</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A98" s="6">
-        <v>1</v>
-      </c>
-      <c r="B98" s="6">
-        <v>1</v>
-      </c>
-      <c r="C98" s="6">
-        <v>0</v>
-      </c>
-      <c r="D98" s="6">
-        <v>0</v>
-      </c>
-      <c r="E98" s="6">
+      <c r="A98">
+        <v>1</v>
+      </c>
+      <c r="B98">
+        <v>1</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98">
         <v>20</v>
       </c>
-      <c r="F98" s="6">
+      <c r="F98">
         <v>2</v>
       </c>
-      <c r="G98" s="6">
-        <v>0</v>
-      </c>
-      <c r="H98" s="6">
+      <c r="G98">
+        <v>0</v>
+      </c>
+      <c r="H98">
         <v>10</v>
       </c>
-      <c r="I98" s="7">
-        <v>1.0000000000000001E-5</v>
+      <c r="I98" s="2">
+        <v>9.9994000359978393E-6</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A99" s="6">
-        <v>1</v>
-      </c>
-      <c r="B99" s="6">
-        <v>1</v>
-      </c>
-      <c r="C99" s="6">
-        <v>0</v>
-      </c>
-      <c r="D99" s="6">
-        <v>0</v>
-      </c>
-      <c r="E99" s="6">
+      <c r="A99">
+        <v>1</v>
+      </c>
+      <c r="B99">
+        <v>1</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
         <v>20</v>
       </c>
-      <c r="F99" s="6">
+      <c r="F99">
         <v>3</v>
       </c>
-      <c r="G99" s="6">
-        <v>0</v>
-      </c>
-      <c r="H99" s="6">
+      <c r="G99">
+        <v>0</v>
+      </c>
+      <c r="H99">
         <v>10</v>
       </c>
-      <c r="I99" s="6">
-        <v>2.9608220000000001E-2</v>
+      <c r="I99">
+        <v>3.0608163510189398E-2</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A100" s="6">
-        <v>1</v>
-      </c>
-      <c r="B100" s="6">
-        <v>1</v>
-      </c>
-      <c r="C100" s="6">
-        <v>0</v>
-      </c>
-      <c r="D100" s="6">
-        <v>0</v>
-      </c>
-      <c r="E100" s="6">
+      <c r="A100">
+        <v>1</v>
+      </c>
+      <c r="B100">
+        <v>1</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100">
         <v>20</v>
       </c>
-      <c r="F100" s="6">
+      <c r="F100">
         <v>4</v>
       </c>
-      <c r="G100" s="6">
-        <v>0</v>
-      </c>
-      <c r="H100" s="6">
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100">
         <v>10</v>
       </c>
-      <c r="I100" s="6">
-        <v>3.0808149999999999E-2</v>
+      <c r="I100">
+        <v>2.87082775033498E-2</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A101" s="6">
-        <v>1</v>
-      </c>
-      <c r="B101" s="6">
-        <v>1</v>
-      </c>
-      <c r="C101" s="6">
-        <v>0</v>
-      </c>
-      <c r="D101" s="6">
-        <v>0</v>
-      </c>
-      <c r="E101" s="6">
+      <c r="A101">
+        <v>1</v>
+      </c>
+      <c r="B101">
+        <v>1</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101">
         <v>20</v>
       </c>
-      <c r="F101" s="6">
+      <c r="F101">
         <v>5</v>
       </c>
-      <c r="G101" s="6">
-        <v>0</v>
-      </c>
-      <c r="H101" s="6">
+      <c r="G101">
+        <v>0</v>
+      </c>
+      <c r="H101">
         <v>10</v>
       </c>
-      <c r="I101" s="6">
-        <v>2.8108310000000001E-2</v>
+      <c r="I101">
+        <v>2.9408235505869702E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Back to no extra SD on survey (better convergence & end of sensitivity)
</commit_message>
<xml_diff>
--- a/data/hake_intrasp_230808_a20.xlsx
+++ b/data/hake_intrasp_230808_a20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93507F40-9DC2-F647-8B27-D10C729470FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510B1767-D6E2-C041-8F1C-3BEE854F67E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6380" yWindow="500" windowWidth="30080" windowHeight="33340" firstSheet="7" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30080" windowHeight="33340" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -1272,7 +1272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1280,7 +1280,6 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -17554,7 +17553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -20755,8 +20754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20788,7 +20787,7 @@
       <c r="G1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="1" t="s">
         <v>171</v>
       </c>
       <c r="I1" s="1" t="s">

</xml_diff>